<commit_message>
back to te begining
</commit_message>
<xml_diff>
--- a/Template_Planilla_Costos.xlsx
+++ b/Template_Planilla_Costos.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desarrollo-RH\Documents\sw-backend-module-prices\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AC3ECodes\19II017-Contract-Plataforma_Interactiva\sw-backend-module-prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8DDA4C3-6896-45A0-BCC7-D4A7F7F6167A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5B3487C-942E-42D4-B2FC-02712BE05E37}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D0EBCE3-B316-476A-AEA7-C8D8F70D0252}"/>
+    <workbookView xWindow="4350" yWindow="5040" windowWidth="13500" windowHeight="8505" xr2:uid="{7D0EBCE3-B316-476A-AEA7-C8D8F70D0252}"/>
   </bookViews>
   <sheets>
     <sheet name="CHILE" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CHILE!$A$1:$F$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">CHILE!$A$1:$F$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="22">
   <si>
     <t>MODULO</t>
   </si>
@@ -103,58 +103,13 @@
   </si>
   <si>
     <t>WYS_PRIVADO_1PERSONA</t>
-  </si>
-  <si>
-    <t>TRAMITACIÓN MUNICIPAL</t>
-  </si>
-  <si>
-    <t>PROYECTOS DE ESPECIALIDADES</t>
-  </si>
-  <si>
-    <t>DIRECCIÓN DE OBRA</t>
-  </si>
-  <si>
-    <t>PROJECT MANAGER</t>
-  </si>
-  <si>
-    <t>INSPECCIÓN TÉCNICA DE OBRA</t>
-  </si>
-  <si>
-    <t>SEGURIDAD E HIGIENE</t>
-  </si>
-  <si>
-    <t>MUDANZA Y GERENCIAMIENTO</t>
-  </si>
-  <si>
-    <t>3,75</t>
-  </si>
-  <si>
-    <t>DEMOLICION</t>
-  </si>
-  <si>
-    <t>BAÑOS NUEVOS</t>
-  </si>
-  <si>
-    <t>BASE CONSTRUCCIÓN</t>
-  </si>
-  <si>
-    <t>por m2</t>
-  </si>
-  <si>
-    <t>por (m2*pisos)</t>
-  </si>
-  <si>
-    <t>por Semana</t>
-  </si>
-  <si>
-    <t>por cada 6,4 m2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,14 +123,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF6600"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,18 +149,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -225,7 +162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -233,12 +170,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -257,7 +188,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -553,24 +484,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C03B4E-5520-41AD-9D0A-6CB3CE544FFF}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D3" sqref="D3:D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="52" customWidth="1"/>
-    <col min="3" max="3" width="35.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" customWidth="1"/>
     <col min="5" max="5" width="22.7109375" customWidth="1"/>
     <col min="6" max="6" width="22.140625" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -590,268 +520,233 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="7">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2">
+        <v>395.4</v>
+      </c>
+      <c r="E2" s="2">
+        <v>395.4</v>
+      </c>
+      <c r="F2" s="2">
+        <v>395.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3">
+        <v>1160.3576470588237</v>
+      </c>
+      <c r="E3" s="3">
+        <v>1571.7576470588233</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1940.5229411764708</v>
+      </c>
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
+        <v>1031.9811764705883</v>
+      </c>
+      <c r="E4" s="3">
+        <v>1624.5524705882353</v>
+      </c>
+      <c r="F4" s="3">
+        <v>6680.162823529412</v>
+      </c>
+      <c r="G4" s="6"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3">
+        <v>284.84823529411761</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3366.3882352941177</v>
+      </c>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3">
+        <v>533.70173935294122</v>
+      </c>
+      <c r="E6" s="3">
+        <v>533.70173935294122</v>
+      </c>
+      <c r="F6" s="3">
+        <v>665.02238647058834</v>
+      </c>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3">
+        <v>145.64582352941176</v>
+      </c>
+      <c r="E7" s="3">
+        <v>145.64582352941176</v>
+      </c>
+      <c r="F7" s="3">
+        <v>206.20664705882356</v>
+      </c>
+      <c r="G7" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3">
+        <v>23.941176470588236</v>
+      </c>
+      <c r="E8" s="3">
+        <v>23.941176470588236</v>
+      </c>
+      <c r="F8" s="3">
+        <v>253.38305882352941</v>
+      </c>
+      <c r="G8" s="6"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3">
+        <v>205.46189529411765</v>
+      </c>
+      <c r="E9" s="3">
+        <v>205.46189529411765</v>
+      </c>
+      <c r="F9" s="3">
+        <v>287.08170441176475</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3">
+        <v>79.583058823529413</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7">
-        <v>10</v>
-      </c>
-      <c r="F2" s="7">
-        <v>10</v>
-      </c>
-      <c r="H2" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="7">
-        <v>10</v>
-      </c>
-      <c r="E3" s="7">
-        <v>10</v>
-      </c>
-      <c r="F3" s="7">
-        <v>10</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D4" s="7">
-        <v>10</v>
-      </c>
-      <c r="E4" s="7">
-        <v>10</v>
-      </c>
-      <c r="F4" s="7">
-        <v>10</v>
-      </c>
-      <c r="G4" s="6"/>
-      <c r="H4" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="I4" s="10"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="7">
-        <v>10</v>
-      </c>
-      <c r="E5" s="7">
-        <v>10</v>
-      </c>
-      <c r="F5" s="7">
-        <v>10</v>
-      </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="I5">
-        <f>950*2.5</f>
-        <v>2375</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="7">
-        <v>10</v>
-      </c>
-      <c r="E6" s="7">
-        <v>10</v>
-      </c>
-      <c r="F6" s="7">
-        <v>10</v>
-      </c>
-      <c r="G6" s="6"/>
-      <c r="H6" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="7">
-        <v>10</v>
-      </c>
-      <c r="E7" s="7">
-        <v>10</v>
-      </c>
-      <c r="F7" s="7">
-        <v>10</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="9" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="7">
-        <v>10</v>
-      </c>
-      <c r="E9" s="7">
-        <v>10</v>
-      </c>
-      <c r="F9" s="7">
-        <v>10</v>
-      </c>
-      <c r="G9" s="6"/>
-      <c r="H9" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="7">
-        <v>10</v>
-      </c>
-      <c r="E10" s="7">
-        <v>10</v>
-      </c>
-      <c r="F10" s="7">
-        <v>10</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D11" s="2">
-        <v>395.4</v>
-      </c>
-      <c r="E11" s="2">
-        <v>395.4</v>
-      </c>
-      <c r="F11" s="2">
-        <v>395.4</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D11" s="3">
+        <v>57.647058823529413</v>
+      </c>
+      <c r="E11" s="3">
+        <v>74.117647058823536</v>
+      </c>
+      <c r="F11" s="3">
+        <v>117.64705882352941</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D12" s="3">
-        <v>57.647058823529413</v>
+        <v>1878.1788235294121</v>
       </c>
       <c r="E12" s="3">
-        <v>74.117647058823536</v>
+        <v>2149.9694117647059</v>
       </c>
       <c r="F12" s="3">
-        <v>117.64705882352941</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+        <v>3133.6994117647059</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
@@ -859,19 +754,19 @@
         <v>19</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D13" s="3">
-        <v>1878.1788235294121</v>
+        <v>1976.675411764706</v>
       </c>
       <c r="E13" s="3">
-        <v>2149.9694117647059</v>
+        <v>2912.383294117647</v>
       </c>
       <c r="F13" s="3">
-        <v>3133.6994117647059</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>11868.016470588236</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>16</v>
       </c>
@@ -879,19 +774,19 @@
         <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D14" s="3">
-        <v>1976.675411764706</v>
+        <v>0</v>
       </c>
       <c r="E14" s="3">
-        <v>2912.383294117647</v>
+        <v>694.82470588235287</v>
       </c>
       <c r="F14" s="3">
-        <v>11868.016470588236</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>8211.5647058823542</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -899,19 +794,19 @@
         <v>19</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D15" s="3">
-        <v>0</v>
+        <v>1093.5910758235295</v>
       </c>
       <c r="E15" s="3">
-        <v>694.82470588235287</v>
+        <v>1093.5910758235295</v>
       </c>
       <c r="F15" s="3">
-        <v>8211.5647058823542</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1413.9189511764707</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -919,16 +814,16 @@
         <v>19</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D16" s="3">
-        <v>1093.5910758235295</v>
+        <v>248.8724117647059</v>
       </c>
       <c r="E16" s="3">
-        <v>1093.5910758235295</v>
+        <v>248.8724117647059</v>
       </c>
       <c r="F16" s="3">
-        <v>1413.9189511764707</v>
+        <v>348.63205882352941</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -939,16 +834,16 @@
         <v>19</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D17" s="3">
-        <v>248.8724117647059</v>
+        <v>23.941176470588236</v>
       </c>
       <c r="E17" s="3">
-        <v>248.8724117647059</v>
+        <v>23.941176470588236</v>
       </c>
       <c r="F17" s="3">
-        <v>348.63205882352941</v>
+        <v>253.38305882352941</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -959,16 +854,16 @@
         <v>19</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D18" s="3">
-        <v>23.941176470588236</v>
+        <v>501.179165882353</v>
       </c>
       <c r="E18" s="3">
-        <v>23.941176470588236</v>
+        <v>501.179165882353</v>
       </c>
       <c r="F18" s="3">
-        <v>253.38305882352941</v>
+        <v>700.27276323529418</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -979,16 +874,16 @@
         <v>19</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D19" s="3">
-        <v>501.179165882353</v>
+        <v>0</v>
       </c>
       <c r="E19" s="3">
-        <v>501.179165882353</v>
+        <v>0</v>
       </c>
       <c r="F19" s="3">
-        <v>700.27276323529418</v>
+        <v>79.583058823529413</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -999,36 +894,36 @@
         <v>19</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D20" s="3">
-        <v>0</v>
+        <v>93.529411764705884</v>
       </c>
       <c r="E20" s="3">
-        <v>0</v>
+        <v>118.82352941176471</v>
       </c>
       <c r="F20" s="3">
-        <v>79.583058823529413</v>
+        <v>195.88235294117646</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="D21" s="3">
-        <v>93.529411764705884</v>
-      </c>
-      <c r="E21" s="3">
-        <v>118.82352941176471</v>
-      </c>
-      <c r="F21" s="3">
-        <v>195.88235294117646</v>
+      <c r="A21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D21" s="5">
+        <v>2631.5105882352937</v>
+      </c>
+      <c r="E21" s="5">
+        <v>3543.7988235294106</v>
+      </c>
+      <c r="F21" s="5">
+        <v>3092.4429411764704</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -1039,16 +934,16 @@
         <v>21</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D22" s="5">
-        <v>2631.5105882352937</v>
+        <v>1224.3957647058824</v>
       </c>
       <c r="E22" s="5">
-        <v>3543.7988235294106</v>
+        <v>1858.9831764705882</v>
       </c>
       <c r="F22" s="5">
-        <v>3092.4429411764704</v>
+        <v>7403.3934117647068</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -1059,16 +954,16 @@
         <v>21</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D23" s="5">
-        <v>1224.3957647058824</v>
+        <v>623.92647058823525</v>
       </c>
       <c r="E23" s="5">
-        <v>1858.9831764705882</v>
+        <v>881.53676470588232</v>
       </c>
       <c r="F23" s="5">
-        <v>7403.3934117647068</v>
+        <v>3919.8144117647057</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -1079,16 +974,16 @@
         <v>21</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D24" s="5">
-        <v>623.92647058823525</v>
+        <v>909.19387058823543</v>
       </c>
       <c r="E24" s="5">
-        <v>881.53676470588232</v>
+        <v>909.19387058823543</v>
       </c>
       <c r="F24" s="5">
-        <v>3919.8144117647057</v>
+        <v>909.19387058823543</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1099,16 +994,16 @@
         <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D25" s="5">
-        <v>909.19387058823543</v>
+        <v>121.42188235294118</v>
       </c>
       <c r="E25" s="5">
-        <v>909.19387058823543</v>
+        <v>121.42188235294118</v>
       </c>
       <c r="F25" s="5">
-        <v>909.19387058823543</v>
+        <v>181.02376470588237</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1119,16 +1014,16 @@
         <v>21</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D26" s="5">
-        <v>121.42188235294118</v>
+        <v>23.941176470588236</v>
       </c>
       <c r="E26" s="5">
-        <v>121.42188235294118</v>
+        <v>47.882352941176471</v>
       </c>
       <c r="F26" s="5">
-        <v>181.02376470588237</v>
+        <v>961.91247058823535</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1139,16 +1034,16 @@
         <v>21</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D27" s="5">
-        <v>23.941176470588236</v>
+        <v>301.8780470588236</v>
       </c>
       <c r="E27" s="5">
-        <v>47.882352941176471</v>
+        <v>301.8780470588236</v>
       </c>
       <c r="F27" s="5">
-        <v>961.91247058823535</v>
+        <v>421.79920588235302</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1159,16 +1054,16 @@
         <v>21</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D28" s="5">
-        <v>301.8780470588236</v>
+        <v>0</v>
       </c>
       <c r="E28" s="5">
-        <v>301.8780470588236</v>
+        <v>55.771294117647059</v>
       </c>
       <c r="F28" s="5">
-        <v>421.79920588235302</v>
+        <v>234.87717647058824</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1179,40 +1074,20 @@
         <v>21</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D29" s="5">
-        <v>0</v>
+        <v>81.17647058823529</v>
       </c>
       <c r="E29" s="5">
-        <v>55.771294117647059</v>
+        <v>121.05882352941177</v>
       </c>
       <c r="F29" s="5">
-        <v>234.87717647058824</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D30" s="5">
-        <v>81.17647058823529</v>
-      </c>
-      <c r="E30" s="5">
-        <v>121.05882352941177</v>
-      </c>
-      <c r="F30" s="5">
         <v>381.41176470588238</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F21" xr:uid="{9B2DB7E7-83C7-49A2-8DA9-FB13A56FD943}"/>
+  <autoFilter ref="A1:F20" xr:uid="{9B2DB7E7-83C7-49A2-8DA9-FB13A56FD943}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Agregada funcionalidad de añadir comentario a PriceCategory
</commit_message>
<xml_diff>
--- a/Template_Planilla_Costos.xlsx
+++ b/Template_Planilla_Costos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\desarrollo-RH\Documents\sw-backend-module-prices\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{752D59F7-2CAA-4AF1-A89E-F0F79309A0A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293F32A5-29B8-4A84-9DE5-2ED464A84C95}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7D0EBCE3-B316-476A-AEA7-C8D8F70D0252}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7D0EBCE3-B316-476A-AEA7-C8D8F70D0252}"/>
   </bookViews>
   <sheets>
     <sheet name="CHILE" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="70">
   <si>
     <t>MODULO</t>
   </si>
@@ -244,6 +244,9 @@
   </si>
   <si>
     <t>WYS_PUESTOTRABAJO_ESTRELLA3PERSONAS</t>
+  </si>
+  <si>
+    <t>CALIDAD_TERMINACIONES</t>
   </si>
 </sst>
 </file>
@@ -656,8 +659,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56C03B4E-5520-41AD-9D0A-6CB3CE544FFF}">
   <dimension ref="A1:J144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F89" sqref="F89"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1146,7 @@
         <v>16</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>42</v>

</xml_diff>